<commit_message>
G# fingerings and Menu
</commit_message>
<xml_diff>
--- a/Sax_details.xlsx
+++ b/Sax_details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim\Documents\GitHub\MIDI-Wind-Controller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6370077D-559F-4FA3-99EE-3360BEB001F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD5B65A-E9F6-4998-8176-73BACA9EB287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21375" yWindow="4275" windowWidth="14040" windowHeight="12735" activeTab="1" xr2:uid="{37DECD7E-2A26-408F-B389-C3EB14E31A56}"/>
+    <workbookView xWindow="7170" yWindow="345" windowWidth="20535" windowHeight="16290" activeTab="1" xr2:uid="{37DECD7E-2A26-408F-B389-C3EB14E31A56}"/>
   </bookViews>
   <sheets>
     <sheet name="Leonardo" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="69">
   <si>
     <t>C#</t>
   </si>
@@ -219,13 +219,37 @@
   </si>
   <si>
     <t>+1 Home Octave With no buttons pressed</t>
+  </si>
+  <si>
+    <t>MODES</t>
+  </si>
+  <si>
+    <t>Semitone Up</t>
+  </si>
+  <si>
+    <t>Semitone Down</t>
+  </si>
+  <si>
+    <t>G# Held down alternative fingerings</t>
+  </si>
+  <si>
+    <t>Enter Menu Mode</t>
+  </si>
+  <si>
+    <t>Leave Menu Mode</t>
+  </si>
+  <si>
+    <t>Concert</t>
+  </si>
+  <si>
+    <t>Eb</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -234,6 +258,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -273,17 +313,179 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -3634,16 +3836,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2919528-146A-CE47-841B-7E3C7B7F9F62}">
-  <dimension ref="A1:W21"/>
+  <dimension ref="A1:W50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="1">
@@ -3756,12 +3958,6 @@
       <c r="Q2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="R2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="T2" s="1"/>
       <c r="V2" s="1" t="s">
         <v>53</v>
@@ -3822,12 +4018,6 @@
       <c r="Q3" s="3">
         <v>1</v>
       </c>
-      <c r="R3" s="3">
-        <v>0</v>
-      </c>
-      <c r="S3" s="3">
-        <v>0</v>
-      </c>
       <c r="T3" s="1" t="s">
         <v>14</v>
       </c>
@@ -3893,12 +4083,6 @@
       <c r="Q4" s="3">
         <v>1</v>
       </c>
-      <c r="R4" s="3">
-        <v>0</v>
-      </c>
-      <c r="S4" s="3">
-        <v>0</v>
-      </c>
       <c r="T4" s="1"/>
       <c r="U4" s="3">
         <v>0</v>
@@ -3962,12 +4146,6 @@
       <c r="Q5" s="3">
         <v>1</v>
       </c>
-      <c r="R5" s="3">
-        <v>0</v>
-      </c>
-      <c r="S5" s="3">
-        <v>0</v>
-      </c>
       <c r="T5" s="1"/>
       <c r="U5" s="3">
         <v>0</v>
@@ -4031,12 +4209,6 @@
       <c r="Q6" s="2">
         <v>0</v>
       </c>
-      <c r="R6" s="2">
-        <v>0</v>
-      </c>
-      <c r="S6" s="2">
-        <v>0</v>
-      </c>
       <c r="T6" s="1"/>
       <c r="U6" s="2">
         <v>0</v>
@@ -4100,12 +4272,6 @@
       <c r="Q7" s="3">
         <v>1</v>
       </c>
-      <c r="R7" s="3">
-        <v>0</v>
-      </c>
-      <c r="S7" s="3">
-        <v>0</v>
-      </c>
       <c r="T7" s="1"/>
       <c r="U7" s="3">
         <v>0</v>
@@ -4169,12 +4335,6 @@
       <c r="Q8" s="3">
         <v>1</v>
       </c>
-      <c r="R8" s="3">
-        <v>0</v>
-      </c>
-      <c r="S8" s="3">
-        <v>0</v>
-      </c>
       <c r="T8" s="1"/>
       <c r="U8" s="3">
         <v>0</v>
@@ -4238,12 +4398,6 @@
       <c r="Q9" s="3">
         <v>1</v>
       </c>
-      <c r="R9" s="3">
-        <v>0</v>
-      </c>
-      <c r="S9" s="3">
-        <v>0</v>
-      </c>
       <c r="T9" s="1"/>
       <c r="U9" s="3">
         <v>0</v>
@@ -4307,12 +4461,6 @@
       <c r="Q10" s="2">
         <v>0</v>
       </c>
-      <c r="R10" s="2">
-        <v>1</v>
-      </c>
-      <c r="S10" s="2">
-        <v>0</v>
-      </c>
       <c r="T10" s="1" t="s">
         <v>15</v>
       </c>
@@ -4378,12 +4526,6 @@
       <c r="Q11" s="2">
         <v>0</v>
       </c>
-      <c r="R11" s="2">
-        <v>0</v>
-      </c>
-      <c r="S11" s="2">
-        <v>0</v>
-      </c>
       <c r="T11" s="1"/>
       <c r="U11" s="2">
         <v>0</v>
@@ -4445,12 +4587,6 @@
         <v>1</v>
       </c>
       <c r="Q12" s="2">
-        <v>1</v>
-      </c>
-      <c r="R12" s="2">
-        <v>0</v>
-      </c>
-      <c r="S12" s="2">
         <v>1</v>
       </c>
       <c r="T12" s="1"/>
@@ -4531,14 +4667,6 @@
       <c r="Q13" s="1">
         <f t="shared" si="0"/>
         <v>631</v>
-      </c>
-      <c r="R13" s="1">
-        <f t="shared" si="0"/>
-        <v>128</v>
-      </c>
-      <c r="S13" s="1">
-        <f t="shared" si="0"/>
-        <v>512</v>
       </c>
       <c r="T13" s="1"/>
       <c r="U13" s="1">
@@ -4547,7 +4675,7 @@
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="5" t="s">
         <v>25</v>
       </c>
       <c r="C16" t="s">
@@ -4557,7 +4685,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>26</v>
       </c>
@@ -4580,7 +4708,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1000</v>
       </c>
@@ -4605,7 +4733,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>10000</v>
       </c>
@@ -4631,7 +4759,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>100000</v>
       </c>
@@ -4657,7 +4785,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D21">
         <v>35</v>
       </c>
@@ -4672,8 +4800,1045 @@
         <v>60</v>
       </c>
     </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="1">
+        <v>49</v>
+      </c>
+      <c r="C24" s="1">
+        <v>48</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1">
+        <v>47</v>
+      </c>
+      <c r="F24" s="1">
+        <v>46</v>
+      </c>
+      <c r="G24" s="1">
+        <v>46</v>
+      </c>
+      <c r="H24" s="1">
+        <v>45</v>
+      </c>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1">
+        <v>42</v>
+      </c>
+      <c r="L24" s="1">
+        <v>41</v>
+      </c>
+      <c r="M24" s="1">
+        <v>40</v>
+      </c>
+      <c r="N24" s="1">
+        <v>39</v>
+      </c>
+      <c r="O24" s="1">
+        <v>38</v>
+      </c>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="2">
+        <v>0</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="3">
+        <v>1</v>
+      </c>
+      <c r="F26" s="3">
+        <v>1</v>
+      </c>
+      <c r="G26" s="3">
+        <v>1</v>
+      </c>
+      <c r="H26" s="3">
+        <v>1</v>
+      </c>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3">
+        <v>1</v>
+      </c>
+      <c r="L26" s="3">
+        <v>1</v>
+      </c>
+      <c r="M26" s="3">
+        <v>1</v>
+      </c>
+      <c r="N26" s="3">
+        <v>1</v>
+      </c>
+      <c r="O26" s="3">
+        <v>1</v>
+      </c>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="2">
+        <v>0</v>
+      </c>
+      <c r="C27" s="3">
+        <v>1</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" s="2">
+        <v>0</v>
+      </c>
+      <c r="F27" s="3">
+        <v>1</v>
+      </c>
+      <c r="G27" s="3">
+        <v>1</v>
+      </c>
+      <c r="H27" s="3">
+        <v>1</v>
+      </c>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3">
+        <v>1</v>
+      </c>
+      <c r="L27" s="3">
+        <v>1</v>
+      </c>
+      <c r="M27" s="3">
+        <v>1</v>
+      </c>
+      <c r="N27" s="3">
+        <v>1</v>
+      </c>
+      <c r="O27" s="3">
+        <v>1</v>
+      </c>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="2">
+        <v>0</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2">
+        <v>0</v>
+      </c>
+      <c r="F28" s="2">
+        <v>0</v>
+      </c>
+      <c r="G28" s="2">
+        <v>0</v>
+      </c>
+      <c r="H28" s="2">
+        <v>0</v>
+      </c>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3">
+        <v>1</v>
+      </c>
+      <c r="L28" s="3">
+        <v>1</v>
+      </c>
+      <c r="M28" s="3">
+        <v>1</v>
+      </c>
+      <c r="N28" s="3">
+        <v>1</v>
+      </c>
+      <c r="O28" s="3">
+        <v>1</v>
+      </c>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="3"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="2">
+        <v>1</v>
+      </c>
+      <c r="C29" s="2">
+        <v>1</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2">
+        <v>1</v>
+      </c>
+      <c r="F29" s="2">
+        <v>1</v>
+      </c>
+      <c r="G29" s="2">
+        <v>1</v>
+      </c>
+      <c r="H29" s="2">
+        <v>1</v>
+      </c>
+      <c r="I29" s="3"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2">
+        <v>1</v>
+      </c>
+      <c r="L29" s="2">
+        <v>1</v>
+      </c>
+      <c r="M29" s="2">
+        <v>1</v>
+      </c>
+      <c r="N29" s="2">
+        <v>1</v>
+      </c>
+      <c r="O29" s="2">
+        <v>1</v>
+      </c>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="2">
+        <v>0</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2">
+        <v>0</v>
+      </c>
+      <c r="F30" s="3">
+        <v>0</v>
+      </c>
+      <c r="G30" s="3">
+        <v>1</v>
+      </c>
+      <c r="H30" s="2">
+        <v>0</v>
+      </c>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2">
+        <v>0</v>
+      </c>
+      <c r="L30" s="3">
+        <v>1</v>
+      </c>
+      <c r="M30" s="3">
+        <v>1</v>
+      </c>
+      <c r="N30" s="3">
+        <v>1</v>
+      </c>
+      <c r="O30" s="3">
+        <v>1</v>
+      </c>
+      <c r="P30" s="3"/>
+      <c r="Q30" s="3"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="2">
+        <v>0</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2">
+        <v>0</v>
+      </c>
+      <c r="F31" s="2">
+        <v>0</v>
+      </c>
+      <c r="G31" s="2">
+        <v>0</v>
+      </c>
+      <c r="H31" s="2">
+        <v>0</v>
+      </c>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="3">
+        <v>1</v>
+      </c>
+      <c r="L31" s="2">
+        <v>0</v>
+      </c>
+      <c r="M31" s="3">
+        <v>1</v>
+      </c>
+      <c r="N31" s="3">
+        <v>1</v>
+      </c>
+      <c r="O31" s="3">
+        <v>1</v>
+      </c>
+      <c r="P31" s="3"/>
+      <c r="Q31" s="3"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="2">
+        <v>0</v>
+      </c>
+      <c r="C32" s="2">
+        <v>0</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2">
+        <v>0</v>
+      </c>
+      <c r="F32" s="2">
+        <v>0</v>
+      </c>
+      <c r="G32" s="2">
+        <v>0</v>
+      </c>
+      <c r="H32" s="2">
+        <v>0</v>
+      </c>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2">
+        <v>0</v>
+      </c>
+      <c r="L32" s="2">
+        <v>0</v>
+      </c>
+      <c r="M32" s="2">
+        <v>0</v>
+      </c>
+      <c r="N32" s="3">
+        <v>1</v>
+      </c>
+      <c r="O32" s="3">
+        <v>1</v>
+      </c>
+      <c r="P32" s="3"/>
+      <c r="Q32" s="3"/>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" s="2">
+        <v>0</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2">
+        <v>0</v>
+      </c>
+      <c r="F33" s="2">
+        <v>0</v>
+      </c>
+      <c r="G33" s="2">
+        <v>0</v>
+      </c>
+      <c r="H33" s="2">
+        <v>0</v>
+      </c>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2">
+        <v>0</v>
+      </c>
+      <c r="L33" s="2">
+        <v>0</v>
+      </c>
+      <c r="M33" s="2">
+        <v>0</v>
+      </c>
+      <c r="N33" s="3">
+        <v>1</v>
+      </c>
+      <c r="O33" s="2">
+        <v>0</v>
+      </c>
+      <c r="P33" s="2"/>
+      <c r="Q33" s="2"/>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34" s="2">
+        <v>0</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0</v>
+      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2">
+        <v>0</v>
+      </c>
+      <c r="F34" s="2">
+        <v>1</v>
+      </c>
+      <c r="G34" s="2">
+        <v>0</v>
+      </c>
+      <c r="H34" s="2">
+        <v>0</v>
+      </c>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2">
+        <v>0</v>
+      </c>
+      <c r="L34" s="2">
+        <v>0</v>
+      </c>
+      <c r="M34" s="2">
+        <v>0</v>
+      </c>
+      <c r="N34" s="3">
+        <v>0</v>
+      </c>
+      <c r="O34" s="2">
+        <v>0</v>
+      </c>
+      <c r="P34" s="2"/>
+      <c r="Q34" s="2"/>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="2">
+        <v>0</v>
+      </c>
+      <c r="C35" s="2">
+        <v>0</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2">
+        <v>0</v>
+      </c>
+      <c r="F35" s="2">
+        <v>0</v>
+      </c>
+      <c r="G35" s="2">
+        <v>0</v>
+      </c>
+      <c r="H35" s="2">
+        <v>0</v>
+      </c>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2">
+        <v>0</v>
+      </c>
+      <c r="L35" s="2">
+        <v>0</v>
+      </c>
+      <c r="M35" s="2">
+        <v>0</v>
+      </c>
+      <c r="N35" s="3">
+        <v>0</v>
+      </c>
+      <c r="O35" s="2">
+        <v>0</v>
+      </c>
+      <c r="P35" s="2"/>
+      <c r="Q35" s="2"/>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" s="1">
+        <f>B26*1+B27*2+B28*4+B29*8+B30*16+B31*32+B32*64+B33*128+B34*256+B35*512</f>
+        <v>8</v>
+      </c>
+      <c r="C36" s="1">
+        <f t="shared" ref="C36:O36" si="2">C26*1+C27*2+C28*4+C29*8+C30*16+C31*32+C32*64+C33*128+C34*256+C35*512</f>
+        <v>10</v>
+      </c>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="F36" s="1">
+        <f t="shared" ref="F36" si="3">F26*1+F27*2+F28*4+F29*8+F30*16+F31*32+F32*64+F33*128+F34*256+F35*512</f>
+        <v>267</v>
+      </c>
+      <c r="G36" s="1">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="H36" s="1">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="L36" s="1">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="M36" s="1">
+        <f t="shared" si="2"/>
+        <v>63</v>
+      </c>
+      <c r="N36" s="1">
+        <f t="shared" si="2"/>
+        <v>255</v>
+      </c>
+      <c r="O36" s="1">
+        <f t="shared" si="2"/>
+        <v>127</v>
+      </c>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="1"/>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40" s="2">
+        <v>0</v>
+      </c>
+      <c r="C40" s="2">
+        <v>0</v>
+      </c>
+      <c r="D40" s="3">
+        <v>0</v>
+      </c>
+      <c r="E40" s="3">
+        <v>0</v>
+      </c>
+      <c r="G40" s="3">
+        <v>0</v>
+      </c>
+      <c r="H40" s="3">
+        <v>0</v>
+      </c>
+      <c r="J40" s="3">
+        <v>1</v>
+      </c>
+      <c r="K40" s="3">
+        <v>0</v>
+      </c>
+      <c r="L40" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" s="2">
+        <v>0</v>
+      </c>
+      <c r="C41" s="2">
+        <v>0</v>
+      </c>
+      <c r="D41" s="3">
+        <v>0</v>
+      </c>
+      <c r="E41" s="3">
+        <v>0</v>
+      </c>
+      <c r="G41" s="3">
+        <v>0</v>
+      </c>
+      <c r="H41" s="3">
+        <v>0</v>
+      </c>
+      <c r="J41" s="3">
+        <v>0</v>
+      </c>
+      <c r="K41" s="3">
+        <v>1</v>
+      </c>
+      <c r="L41" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" s="2">
+        <v>0</v>
+      </c>
+      <c r="C42" s="2">
+        <v>0</v>
+      </c>
+      <c r="D42" s="3">
+        <v>0</v>
+      </c>
+      <c r="E42" s="3">
+        <v>0</v>
+      </c>
+      <c r="G42" s="3">
+        <v>0</v>
+      </c>
+      <c r="H42" s="3">
+        <v>0</v>
+      </c>
+      <c r="J42" s="3">
+        <v>0</v>
+      </c>
+      <c r="K42" s="3">
+        <v>0</v>
+      </c>
+      <c r="L42" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" s="2">
+        <v>0</v>
+      </c>
+      <c r="C43" s="2">
+        <v>0</v>
+      </c>
+      <c r="D43" s="2">
+        <v>0</v>
+      </c>
+      <c r="E43" s="2">
+        <v>0</v>
+      </c>
+      <c r="G43" s="2">
+        <v>1</v>
+      </c>
+      <c r="H43" s="2">
+        <v>0</v>
+      </c>
+      <c r="J43" s="2">
+        <v>0</v>
+      </c>
+      <c r="K43" s="2">
+        <v>0</v>
+      </c>
+      <c r="L43" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" s="2">
+        <v>0</v>
+      </c>
+      <c r="C44" s="2">
+        <v>0</v>
+      </c>
+      <c r="D44" s="3">
+        <v>0</v>
+      </c>
+      <c r="E44" s="3">
+        <v>0</v>
+      </c>
+      <c r="G44" s="3">
+        <v>0</v>
+      </c>
+      <c r="H44" s="3">
+        <v>0</v>
+      </c>
+      <c r="J44" s="3">
+        <v>0</v>
+      </c>
+      <c r="K44" s="3">
+        <v>0</v>
+      </c>
+      <c r="L44" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B45" s="2">
+        <v>0</v>
+      </c>
+      <c r="C45" s="2">
+        <v>0</v>
+      </c>
+      <c r="D45" s="3">
+        <v>0</v>
+      </c>
+      <c r="E45" s="3">
+        <v>0</v>
+      </c>
+      <c r="G45" s="3">
+        <v>0</v>
+      </c>
+      <c r="H45" s="3">
+        <v>0</v>
+      </c>
+      <c r="J45" s="3">
+        <v>0</v>
+      </c>
+      <c r="K45" s="3">
+        <v>0</v>
+      </c>
+      <c r="L45" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B46" s="2">
+        <v>0</v>
+      </c>
+      <c r="C46" s="2">
+        <v>1</v>
+      </c>
+      <c r="D46" s="3">
+        <v>0</v>
+      </c>
+      <c r="E46" s="3">
+        <v>0</v>
+      </c>
+      <c r="G46" s="3">
+        <v>0</v>
+      </c>
+      <c r="H46" s="3">
+        <v>0</v>
+      </c>
+      <c r="J46" s="3">
+        <v>0</v>
+      </c>
+      <c r="K46" s="3">
+        <v>0</v>
+      </c>
+      <c r="L46" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47" s="2">
+        <v>1</v>
+      </c>
+      <c r="C47" s="2">
+        <v>0</v>
+      </c>
+      <c r="D47" s="2">
+        <v>1</v>
+      </c>
+      <c r="E47" s="2">
+        <v>0</v>
+      </c>
+      <c r="G47" s="2">
+        <v>0</v>
+      </c>
+      <c r="H47" s="2">
+        <v>0</v>
+      </c>
+      <c r="J47" s="2">
+        <v>0</v>
+      </c>
+      <c r="K47" s="2">
+        <v>0</v>
+      </c>
+      <c r="L47" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B48" s="2">
+        <v>0</v>
+      </c>
+      <c r="C48" s="2">
+        <v>0</v>
+      </c>
+      <c r="D48" s="2">
+        <v>0</v>
+      </c>
+      <c r="E48" s="2">
+        <v>0</v>
+      </c>
+      <c r="G48" s="2">
+        <v>0</v>
+      </c>
+      <c r="H48" s="2">
+        <v>1</v>
+      </c>
+      <c r="J48" s="2">
+        <v>0</v>
+      </c>
+      <c r="K48" s="2">
+        <v>0</v>
+      </c>
+      <c r="L48" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B49" s="2">
+        <v>1</v>
+      </c>
+      <c r="C49" s="2">
+        <v>0</v>
+      </c>
+      <c r="D49" s="2">
+        <v>0</v>
+      </c>
+      <c r="E49" s="2">
+        <v>1</v>
+      </c>
+      <c r="G49" s="2">
+        <v>0</v>
+      </c>
+      <c r="H49" s="2">
+        <v>0</v>
+      </c>
+      <c r="J49" s="2">
+        <v>0</v>
+      </c>
+      <c r="K49" s="2">
+        <v>0</v>
+      </c>
+      <c r="L49" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B50" s="1">
+        <f>B40*1+B41*2+B42*4+B43*8+B44*16+B45*32+B46*64+B47*128+B48*256+B49*512</f>
+        <v>640</v>
+      </c>
+      <c r="C50" s="1">
+        <f>C40*1+C41*2+C42*4+C43*8+C44*16+C45*32+C46*64+C47*128+C48*256+C49*512</f>
+        <v>64</v>
+      </c>
+      <c r="D50" s="1">
+        <f>D40*1+D41*2+D42*4+D43*8+D44*16+D45*32+D46*64+D47*128+D48*256+D49*512</f>
+        <v>128</v>
+      </c>
+      <c r="E50" s="1">
+        <f>E40*1+E41*2+E42*4+E43*8+E44*16+E45*32+E46*64+E47*128+E48*256+E49*512</f>
+        <v>512</v>
+      </c>
+      <c r="G50" s="1">
+        <f>G40*1+G41*2+G42*4+G43*8+G44*16+G45*32+G46*64+G47*128+G48*256+G49*512</f>
+        <v>8</v>
+      </c>
+      <c r="H50" s="1">
+        <f>H40*1+H41*2+H42*4+H43*8+H44*16+H45*32+H46*64+H47*128+H48*256+H49*512</f>
+        <v>256</v>
+      </c>
+      <c r="J50" s="1">
+        <f>J40*1+J41*2+J42*4+J43*8+J44*16+J45*32+J46*64+J47*128+J48*256+J49*512</f>
+        <v>1</v>
+      </c>
+      <c r="K50" s="1">
+        <f>K40*1+K41*2+K42*4+K43*8+K44*16+K45*32+K46*64+K47*128+K48*256+K49*512</f>
+        <v>2</v>
+      </c>
+      <c r="L50" s="1">
+        <f>L40*1+L41*2+L42*4+L43*8+L44*16+L45*32+L46*64+L47*128+L48*256+L49*512</f>
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:S12 U3:U12">
+  <conditionalFormatting sqref="U3:U12 B3:Q12 D40:E49">
+    <cfRule type="cellIs" dxfId="17" priority="19" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="20" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B26:E35 G26:Q35">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B40:B49">
+    <cfRule type="cellIs" dxfId="13" priority="13" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G40:H49">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J40:J49">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C40:C49">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F26:F35">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K40:K49">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L40:L49">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>1</formula>
     </cfRule>
@@ -4682,6 +5847,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>